<commit_message>
fixade vasi-stats i finalen
</commit_message>
<xml_diff>
--- a/2018/static/games/R1/G2/NHLFantasyDraft201819.xlsx
+++ b/2018/static/games/R1/G2/NHLFantasyDraft201819.xlsx
@@ -743,9 +743,6 @@
     <t>Fleury</t>
   </si>
   <si>
-    <t>Markström</t>
-  </si>
-  <si>
     <t>Holtby</t>
   </si>
   <si>
@@ -807,6 +804,9 @@
   </si>
   <si>
     <t>Thornton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1854,10 +1854,10 @@
         <v>234</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>1</v>
@@ -1904,10 +1904,10 @@
         <v>181</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>1</v>
@@ -1954,10 +1954,10 @@
         <v>65</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>1</v>
@@ -1998,10 +1998,10 @@
         <v>236</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>1</v>
@@ -2021,7 +2021,7 @@
         <v>189</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>207</v>
@@ -2033,10 +2033,10 @@
         <v>235</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>1</v>
@@ -2056,10 +2056,10 @@
         <v>219</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>1</v>
@@ -2129,10 +2129,10 @@
         <v>237</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>2</v>
@@ -2173,10 +2173,10 @@
         <v>217</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>2</v>
@@ -2199,10 +2199,10 @@
         <v>222</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>2</v>
@@ -2277,16 +2277,16 @@
         <v>229</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>238</v>
       </c>
       <c r="O29" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="P29" s="7" t="s">
         <v>240</v>
-      </c>
-      <c r="P29" s="7" t="s">
-        <v>241</v>
       </c>
       <c r="R29" s="2" t="s">
         <v>33</v>

</xml_diff>